<commit_message>
simple graph added, requires small fixes. added todo tasks
</commit_message>
<xml_diff>
--- a/DataBase/GDN_Arrivals.xlsx
+++ b/DataBase/GDN_Arrivals.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4027" uniqueCount="862">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4187" uniqueCount="878">
   <si>
     <t>NUMBER</t>
   </si>
@@ -2598,6 +2598,54 @@
   </si>
   <si>
     <t>(VRN)</t>
+  </si>
+  <si>
+    <t>5:57 PM</t>
+  </si>
+  <si>
+    <t>(9H-LOS)</t>
+  </si>
+  <si>
+    <t>6:47 PM</t>
+  </si>
+  <si>
+    <t>8:13 PM</t>
+  </si>
+  <si>
+    <t>0 hours, 53 minutes</t>
+  </si>
+  <si>
+    <t>8:25 PM</t>
+  </si>
+  <si>
+    <t>8:22 PM</t>
+  </si>
+  <si>
+    <t>8:18 PM</t>
+  </si>
+  <si>
+    <t>8:43 PM</t>
+  </si>
+  <si>
+    <t>(D-ACKH)</t>
+  </si>
+  <si>
+    <t>9:54 PM</t>
+  </si>
+  <si>
+    <t>0 hours, 25 minutes</t>
+  </si>
+  <si>
+    <t>11:53 PM</t>
+  </si>
+  <si>
+    <t>11:23 PM</t>
+  </si>
+  <si>
+    <t>Sunday, Jan 15</t>
+  </si>
+  <si>
+    <t>23 hours, 50 minutes</t>
   </si>
 </sst>
 </file>
@@ -2642,7 +2690,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M403"/>
+  <dimension ref="A1:M419"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -17549,6 +17597,598 @@
       </c>
       <c r="M403" s="0"/>
     </row>
+    <row r="404">
+      <c r="A404" t="n" s="0">
+        <v>403.0</v>
+      </c>
+      <c r="B404" t="s" s="0">
+        <v>830</v>
+      </c>
+      <c r="C404" t="s" s="0">
+        <v>193</v>
+      </c>
+      <c r="D404" t="s" s="0">
+        <v>194</v>
+      </c>
+      <c r="E404" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="F404" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="G404" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="H404" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I404" t="s" s="0">
+        <v>720</v>
+      </c>
+      <c r="J404" t="s" s="0">
+        <v>862</v>
+      </c>
+      <c r="K404" s="0"/>
+      <c r="L404" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="M404" s="0"/>
+    </row>
+    <row r="405">
+      <c r="A405" t="n" s="0">
+        <v>404.0</v>
+      </c>
+      <c r="B405" t="s" s="0">
+        <v>830</v>
+      </c>
+      <c r="C405" t="s" s="0">
+        <v>197</v>
+      </c>
+      <c r="D405" t="s" s="0">
+        <v>198</v>
+      </c>
+      <c r="E405" t="s" s="0">
+        <v>199</v>
+      </c>
+      <c r="F405" t="s" s="0">
+        <v>200</v>
+      </c>
+      <c r="G405" t="s" s="0">
+        <v>201</v>
+      </c>
+      <c r="H405" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="I405" t="s" s="0">
+        <v>863</v>
+      </c>
+      <c r="J405" t="s" s="0">
+        <v>864</v>
+      </c>
+      <c r="K405" s="0"/>
+      <c r="L405" t="s" s="0">
+        <v>247</v>
+      </c>
+      <c r="M405" s="0"/>
+    </row>
+    <row r="406">
+      <c r="A406" t="n" s="0">
+        <v>405.0</v>
+      </c>
+      <c r="B406" t="s" s="0">
+        <v>830</v>
+      </c>
+      <c r="C406" t="s" s="0">
+        <v>204</v>
+      </c>
+      <c r="D406" t="s" s="0">
+        <v>205</v>
+      </c>
+      <c r="E406" t="s" s="0">
+        <v>206</v>
+      </c>
+      <c r="F406" t="s" s="0">
+        <v>207</v>
+      </c>
+      <c r="G406" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="H406" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="I406" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="J406" t="s" s="0">
+        <v>865</v>
+      </c>
+      <c r="K406" s="0"/>
+      <c r="L406" t="s" s="0">
+        <v>866</v>
+      </c>
+      <c r="M406" s="0"/>
+    </row>
+    <row r="407">
+      <c r="A407" t="n" s="0">
+        <v>406.0</v>
+      </c>
+      <c r="B407" t="s" s="0">
+        <v>830</v>
+      </c>
+      <c r="C407" t="s" s="0">
+        <v>867</v>
+      </c>
+      <c r="D407" t="s" s="0">
+        <v>211</v>
+      </c>
+      <c r="E407" t="s" s="0">
+        <v>212</v>
+      </c>
+      <c r="F407" t="s" s="0">
+        <v>213</v>
+      </c>
+      <c r="G407" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="H407" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="I407" t="s" s="0">
+        <v>793</v>
+      </c>
+      <c r="J407" t="s" s="0">
+        <v>868</v>
+      </c>
+      <c r="K407" s="0"/>
+      <c r="L407" t="s" s="0">
+        <v>181</v>
+      </c>
+      <c r="M407" s="0"/>
+    </row>
+    <row r="408">
+      <c r="A408" t="n" s="0">
+        <v>407.0</v>
+      </c>
+      <c r="B408" t="s" s="0">
+        <v>830</v>
+      </c>
+      <c r="C408" t="s" s="0">
+        <v>221</v>
+      </c>
+      <c r="D408" t="s" s="0">
+        <v>222</v>
+      </c>
+      <c r="E408" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="F408" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="G408" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="H408" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I408" t="s" s="0">
+        <v>348</v>
+      </c>
+      <c r="J408" t="s" s="0">
+        <v>869</v>
+      </c>
+      <c r="K408" s="0"/>
+      <c r="L408" t="s" s="0">
+        <v>287</v>
+      </c>
+      <c r="M408" s="0"/>
+    </row>
+    <row r="409">
+      <c r="A409" t="n" s="0">
+        <v>408.0</v>
+      </c>
+      <c r="B409" t="s" s="0">
+        <v>830</v>
+      </c>
+      <c r="C409" t="s" s="0">
+        <v>225</v>
+      </c>
+      <c r="D409" t="s" s="0">
+        <v>226</v>
+      </c>
+      <c r="E409" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F409" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="G409" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="H409" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="I409" t="s" s="0">
+        <v>840</v>
+      </c>
+      <c r="J409" t="s" s="0">
+        <v>870</v>
+      </c>
+      <c r="K409" s="0"/>
+      <c r="L409" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="M409" s="0"/>
+    </row>
+    <row r="410">
+      <c r="A410" t="n" s="0">
+        <v>409.0</v>
+      </c>
+      <c r="B410" t="s" s="0">
+        <v>830</v>
+      </c>
+      <c r="C410" t="s" s="0">
+        <v>228</v>
+      </c>
+      <c r="D410" t="s" s="0">
+        <v>229</v>
+      </c>
+      <c r="E410" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="F410" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="G410" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="H410" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="I410" t="s" s="0">
+        <v>871</v>
+      </c>
+      <c r="J410" t="s" s="0">
+        <v>628</v>
+      </c>
+      <c r="K410" s="0"/>
+      <c r="L410" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="M410" s="0"/>
+    </row>
+    <row r="411">
+      <c r="A411" t="n" s="0">
+        <v>410.0</v>
+      </c>
+      <c r="B411" t="s" s="0">
+        <v>830</v>
+      </c>
+      <c r="C411" t="s" s="0">
+        <v>413</v>
+      </c>
+      <c r="D411" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="E411" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="F411" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="G411" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="H411" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="I411" t="s" s="0">
+        <v>135</v>
+      </c>
+      <c r="J411" t="s" s="0">
+        <v>872</v>
+      </c>
+      <c r="K411" s="0"/>
+      <c r="L411" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="M411" s="0"/>
+    </row>
+    <row r="412">
+      <c r="A412" t="n" s="0">
+        <v>411.0</v>
+      </c>
+      <c r="B412" t="s" s="0">
+        <v>830</v>
+      </c>
+      <c r="C412" t="s" s="0">
+        <v>248</v>
+      </c>
+      <c r="D412" t="s" s="0">
+        <v>249</v>
+      </c>
+      <c r="E412" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="F412" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="G412" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="H412" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I412" t="s" s="0">
+        <v>720</v>
+      </c>
+      <c r="J412" t="s" s="0">
+        <v>760</v>
+      </c>
+      <c r="K412" s="0"/>
+      <c r="L412" t="s" s="0">
+        <v>873</v>
+      </c>
+      <c r="M412" s="0"/>
+    </row>
+    <row r="413">
+      <c r="A413" t="n" s="0">
+        <v>412.0</v>
+      </c>
+      <c r="B413" t="s" s="0">
+        <v>830</v>
+      </c>
+      <c r="C413" t="s" s="0">
+        <v>252</v>
+      </c>
+      <c r="D413" t="s" s="0">
+        <v>253</v>
+      </c>
+      <c r="E413" t="s" s="0">
+        <v>254</v>
+      </c>
+      <c r="F413" t="s" s="0">
+        <v>255</v>
+      </c>
+      <c r="G413" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="H413" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I413" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="J413" t="s" s="0">
+        <v>435</v>
+      </c>
+      <c r="K413" s="0"/>
+      <c r="L413" t="s" s="0">
+        <v>821</v>
+      </c>
+      <c r="M413" s="0"/>
+    </row>
+    <row r="414">
+      <c r="A414" t="n" s="0">
+        <v>413.0</v>
+      </c>
+      <c r="B414" t="s" s="0">
+        <v>830</v>
+      </c>
+      <c r="C414" t="s" s="0">
+        <v>427</v>
+      </c>
+      <c r="D414" t="s" s="0">
+        <v>646</v>
+      </c>
+      <c r="E414" t="s" s="0">
+        <v>647</v>
+      </c>
+      <c r="F414" t="s" s="0">
+        <v>648</v>
+      </c>
+      <c r="G414" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="H414" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="I414" t="s" s="0">
+        <v>156</v>
+      </c>
+      <c r="J414" t="s" s="0">
+        <v>428</v>
+      </c>
+      <c r="K414" s="0"/>
+      <c r="L414" t="s" s="0">
+        <v>257</v>
+      </c>
+      <c r="M414" s="0"/>
+    </row>
+    <row r="415">
+      <c r="A415" t="n" s="0">
+        <v>414.0</v>
+      </c>
+      <c r="B415" t="s" s="0">
+        <v>830</v>
+      </c>
+      <c r="C415" t="s" s="0">
+        <v>427</v>
+      </c>
+      <c r="D415" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="E415" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="F415" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="G415" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="H415" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="I415" t="s" s="0">
+        <v>762</v>
+      </c>
+      <c r="J415" t="s" s="0">
+        <v>874</v>
+      </c>
+      <c r="K415" s="0"/>
+      <c r="L415" t="s" s="0">
+        <v>686</v>
+      </c>
+      <c r="M415" s="0"/>
+    </row>
+    <row r="416">
+      <c r="A416" t="n" s="0">
+        <v>415.0</v>
+      </c>
+      <c r="B416" t="s" s="0">
+        <v>830</v>
+      </c>
+      <c r="C416" t="s" s="0">
+        <v>258</v>
+      </c>
+      <c r="D416" t="s" s="0">
+        <v>259</v>
+      </c>
+      <c r="E416" t="s" s="0">
+        <v>260</v>
+      </c>
+      <c r="F416" t="s" s="0">
+        <v>261</v>
+      </c>
+      <c r="G416" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="H416" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I416" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="J416" t="s" s="0">
+        <v>875</v>
+      </c>
+      <c r="K416" s="0"/>
+      <c r="L416" t="s" s="0">
+        <v>465</v>
+      </c>
+      <c r="M416" s="0"/>
+    </row>
+    <row r="417">
+      <c r="A417" t="n" s="0">
+        <v>416.0</v>
+      </c>
+      <c r="B417" t="s" s="0">
+        <v>830</v>
+      </c>
+      <c r="C417" t="s" s="0">
+        <v>258</v>
+      </c>
+      <c r="D417" t="s" s="0">
+        <v>263</v>
+      </c>
+      <c r="E417" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="F417" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="G417" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="H417" t="s" s="0">
+        <v>616</v>
+      </c>
+      <c r="I417" t="s" s="0">
+        <v>639</v>
+      </c>
+      <c r="J417" t="s" s="0">
+        <v>633</v>
+      </c>
+      <c r="K417" s="0"/>
+      <c r="L417" t="s" s="0">
+        <v>662</v>
+      </c>
+      <c r="M417" s="0"/>
+    </row>
+    <row r="418">
+      <c r="A418" t="n" s="0">
+        <v>417.0</v>
+      </c>
+      <c r="B418" t="s" s="0">
+        <v>830</v>
+      </c>
+      <c r="C418" t="s" s="0">
+        <v>266</v>
+      </c>
+      <c r="D418" t="s" s="0">
+        <v>267</v>
+      </c>
+      <c r="E418" t="s" s="0">
+        <v>268</v>
+      </c>
+      <c r="F418" t="s" s="0">
+        <v>269</v>
+      </c>
+      <c r="G418" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="H418" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I418" t="s" s="0">
+        <v>186</v>
+      </c>
+      <c r="J418" t="s" s="0">
+        <v>429</v>
+      </c>
+      <c r="K418" s="0"/>
+      <c r="L418" t="s" s="0">
+        <v>344</v>
+      </c>
+      <c r="M418" s="0"/>
+    </row>
+    <row r="419">
+      <c r="A419" t="n" s="0">
+        <v>418.0</v>
+      </c>
+      <c r="B419" t="s" s="0">
+        <v>876</v>
+      </c>
+      <c r="C419" t="s" s="0">
+        <v>277</v>
+      </c>
+      <c r="D419" t="s" s="0">
+        <v>278</v>
+      </c>
+      <c r="E419" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F419" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="G419" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="H419" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="I419" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="J419" t="s" s="0">
+        <v>272</v>
+      </c>
+      <c r="K419" s="0"/>
+      <c r="L419" t="s" s="0">
+        <v>877</v>
+      </c>
+      <c r="M419" s="0"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
all graphs added and working, deleted and renamed files
</commit_message>
<xml_diff>
--- a/DataBase/GDN_Arrivals.xlsx
+++ b/DataBase/GDN_Arrivals.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4387" uniqueCount="893">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4427" uniqueCount="895">
   <si>
     <t>NUMBER</t>
   </si>
@@ -2691,6 +2691,12 @@
   </si>
   <si>
     <t>3:46 PM</t>
+  </si>
+  <si>
+    <t>(PH-EZF)</t>
+  </si>
+  <si>
+    <t>5:25 PM</t>
   </si>
 </sst>
 </file>
@@ -2735,7 +2741,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M439"/>
+  <dimension ref="A1:M443"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -18974,6 +18980,154 @@
       </c>
       <c r="M439" s="0"/>
     </row>
+    <row r="440">
+      <c r="A440" t="n" s="0">
+        <v>439.0</v>
+      </c>
+      <c r="B440" t="s" s="0">
+        <v>876</v>
+      </c>
+      <c r="C440" t="s" s="0">
+        <v>159</v>
+      </c>
+      <c r="D440" t="s" s="0">
+        <v>160</v>
+      </c>
+      <c r="E440" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F440" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="G440" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="H440" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="I440" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="J440" t="s" s="0">
+        <v>512</v>
+      </c>
+      <c r="K440" s="0"/>
+      <c r="L440" t="s" s="0">
+        <v>364</v>
+      </c>
+      <c r="M440" s="0"/>
+    </row>
+    <row r="441">
+      <c r="A441" t="n" s="0">
+        <v>440.0</v>
+      </c>
+      <c r="B441" t="s" s="0">
+        <v>876</v>
+      </c>
+      <c r="C441" t="s" s="0">
+        <v>159</v>
+      </c>
+      <c r="D441" t="s" s="0">
+        <v>237</v>
+      </c>
+      <c r="E441" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="F441" t="s" s="0">
+        <v>239</v>
+      </c>
+      <c r="G441" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="H441" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="I441" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="J441" t="s" s="0">
+        <v>159</v>
+      </c>
+      <c r="K441" s="0"/>
+      <c r="L441" t="s" s="0">
+        <v>141</v>
+      </c>
+      <c r="M441" s="0"/>
+    </row>
+    <row r="442">
+      <c r="A442" t="n" s="0">
+        <v>441.0</v>
+      </c>
+      <c r="B442" t="s" s="0">
+        <v>876</v>
+      </c>
+      <c r="C442" t="s" s="0">
+        <v>192</v>
+      </c>
+      <c r="D442" t="s" s="0">
+        <v>378</v>
+      </c>
+      <c r="E442" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="F442" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="G442" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="H442" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="I442" t="s" s="0">
+        <v>893</v>
+      </c>
+      <c r="J442" t="s" s="0">
+        <v>521</v>
+      </c>
+      <c r="K442" s="0"/>
+      <c r="L442" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="M442" s="0"/>
+    </row>
+    <row r="443">
+      <c r="A443" t="n" s="0">
+        <v>442.0</v>
+      </c>
+      <c r="B443" t="s" s="0">
+        <v>876</v>
+      </c>
+      <c r="C443" t="s" s="0">
+        <v>192</v>
+      </c>
+      <c r="D443" t="s" s="0">
+        <v>176</v>
+      </c>
+      <c r="E443" t="s" s="0">
+        <v>177</v>
+      </c>
+      <c r="F443" t="s" s="0">
+        <v>178</v>
+      </c>
+      <c r="G443" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="H443" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="I443" t="s" s="0">
+        <v>156</v>
+      </c>
+      <c r="J443" t="s" s="0">
+        <v>894</v>
+      </c>
+      <c r="K443" s="0"/>
+      <c r="L443" t="s" s="0">
+        <v>442</v>
+      </c>
+      <c r="M443" s="0"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
5.0 project passed :)
</commit_message>
<xml_diff>
--- a/DataBase/GDN_Arrivals.xlsx
+++ b/DataBase/GDN_Arrivals.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4647" uniqueCount="916">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4737" uniqueCount="926">
   <si>
     <t>NUMBER</t>
   </si>
@@ -2760,6 +2760,36 @@
   </si>
   <si>
     <t>23 hours, 44 minutes</t>
+  </si>
+  <si>
+    <t>QY5102</t>
+  </si>
+  <si>
+    <t>1:53 AM</t>
+  </si>
+  <si>
+    <t>6:04 AM</t>
+  </si>
+  <si>
+    <t>Katowice</t>
+  </si>
+  <si>
+    <t>(KTW)</t>
+  </si>
+  <si>
+    <t>7:29 AM</t>
+  </si>
+  <si>
+    <t>7:34 AM</t>
+  </si>
+  <si>
+    <t>9:33 AM</t>
+  </si>
+  <si>
+    <t>9:16 AM</t>
+  </si>
+  <si>
+    <t>10:11 AM</t>
   </si>
 </sst>
 </file>
@@ -2804,7 +2834,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M465"/>
+  <dimension ref="A1:M474"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -20005,6 +20035,339 @@
       </c>
       <c r="M465" s="0"/>
     </row>
+    <row r="466">
+      <c r="A466" t="n" s="0">
+        <v>465.0</v>
+      </c>
+      <c r="B466" t="s" s="0">
+        <v>913</v>
+      </c>
+      <c r="C466" t="s" s="0">
+        <v>450</v>
+      </c>
+      <c r="D466" t="s" s="0">
+        <v>916</v>
+      </c>
+      <c r="E466" t="s" s="0">
+        <v>451</v>
+      </c>
+      <c r="F466" t="s" s="0">
+        <v>452</v>
+      </c>
+      <c r="G466" t="s" s="0">
+        <v>453</v>
+      </c>
+      <c r="H466" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I466" t="s" s="0">
+        <v>454</v>
+      </c>
+      <c r="J466" t="s" s="0">
+        <v>917</v>
+      </c>
+      <c r="K466" s="0"/>
+      <c r="L466" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="M466" s="0"/>
+    </row>
+    <row r="467">
+      <c r="A467" t="n" s="0">
+        <v>466.0</v>
+      </c>
+      <c r="B467" t="s" s="0">
+        <v>913</v>
+      </c>
+      <c r="C467" t="s" s="0">
+        <v>918</v>
+      </c>
+      <c r="D467" t="s" s="0">
+        <v>183</v>
+      </c>
+      <c r="E467" t="s" s="0">
+        <v>919</v>
+      </c>
+      <c r="F467" t="s" s="0">
+        <v>920</v>
+      </c>
+      <c r="G467" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="H467" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I467" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="J467" t="s" s="0">
+        <v>918</v>
+      </c>
+      <c r="K467" s="0"/>
+      <c r="L467" t="s" s="0">
+        <v>141</v>
+      </c>
+      <c r="M467" s="0"/>
+    </row>
+    <row r="468">
+      <c r="A468" t="n" s="0">
+        <v>467.0</v>
+      </c>
+      <c r="B468" t="s" s="0">
+        <v>913</v>
+      </c>
+      <c r="C468" t="s" s="0">
+        <v>456</v>
+      </c>
+      <c r="D468" t="s" s="0">
+        <v>345</v>
+      </c>
+      <c r="E468" t="s" s="0">
+        <v>346</v>
+      </c>
+      <c r="F468" t="s" s="0">
+        <v>347</v>
+      </c>
+      <c r="G468" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="H468" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I468" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="J468" t="s" s="0">
+        <v>921</v>
+      </c>
+      <c r="K468" s="0"/>
+      <c r="L468" t="s" s="0">
+        <v>423</v>
+      </c>
+      <c r="M468" s="0"/>
+    </row>
+    <row r="469">
+      <c r="A469" t="n" s="0">
+        <v>468.0</v>
+      </c>
+      <c r="B469" t="s" s="0">
+        <v>913</v>
+      </c>
+      <c r="C469" t="s" s="0">
+        <v>458</v>
+      </c>
+      <c r="D469" t="s" s="0">
+        <v>497</v>
+      </c>
+      <c r="E469" t="s" s="0">
+        <v>206</v>
+      </c>
+      <c r="F469" t="s" s="0">
+        <v>207</v>
+      </c>
+      <c r="G469" t="s" s="0">
+        <v>500</v>
+      </c>
+      <c r="H469" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="I469" t="s" s="0">
+        <v>771</v>
+      </c>
+      <c r="J469" t="s" s="0">
+        <v>922</v>
+      </c>
+      <c r="K469" s="0"/>
+      <c r="L469" t="s" s="0">
+        <v>275</v>
+      </c>
+      <c r="M469" s="0"/>
+    </row>
+    <row r="470">
+      <c r="A470" t="n" s="0">
+        <v>469.0</v>
+      </c>
+      <c r="B470" t="s" s="0">
+        <v>913</v>
+      </c>
+      <c r="C470" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="D470" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="E470" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="F470" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="G470" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="H470" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I470" t="s" s="0">
+        <v>720</v>
+      </c>
+      <c r="J470" t="s" s="0">
+        <v>923</v>
+      </c>
+      <c r="K470" s="0"/>
+      <c r="L470" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="M470" s="0"/>
+    </row>
+    <row r="471">
+      <c r="A471" t="n" s="0">
+        <v>470.0</v>
+      </c>
+      <c r="B471" t="s" s="0">
+        <v>913</v>
+      </c>
+      <c r="C471" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="D471" t="s" s="0">
+        <v>324</v>
+      </c>
+      <c r="E471" t="s" s="0">
+        <v>325</v>
+      </c>
+      <c r="F471" t="s" s="0">
+        <v>326</v>
+      </c>
+      <c r="G471" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="H471" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I471" t="s" s="0">
+        <v>186</v>
+      </c>
+      <c r="J471" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="K471" s="0"/>
+      <c r="L471" t="s" s="0">
+        <v>181</v>
+      </c>
+      <c r="M471" s="0"/>
+    </row>
+    <row r="472">
+      <c r="A472" t="n" s="0">
+        <v>471.0</v>
+      </c>
+      <c r="B472" t="s" s="0">
+        <v>913</v>
+      </c>
+      <c r="C472" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="D472" t="s" s="0">
+        <v>461</v>
+      </c>
+      <c r="E472" t="s" s="0">
+        <v>462</v>
+      </c>
+      <c r="F472" t="s" s="0">
+        <v>463</v>
+      </c>
+      <c r="G472" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="H472" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I472" t="s" s="0">
+        <v>348</v>
+      </c>
+      <c r="J472" t="s" s="0">
+        <v>924</v>
+      </c>
+      <c r="K472" s="0"/>
+      <c r="L472" t="s" s="0">
+        <v>174</v>
+      </c>
+      <c r="M472" s="0"/>
+    </row>
+    <row r="473">
+      <c r="A473" t="n" s="0">
+        <v>472.0</v>
+      </c>
+      <c r="B473" t="s" s="0">
+        <v>913</v>
+      </c>
+      <c r="C473" t="s" s="0">
+        <v>466</v>
+      </c>
+      <c r="D473" t="s" s="0">
+        <v>467</v>
+      </c>
+      <c r="E473" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F473" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="G473" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="H473" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I473" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="J473" t="s" s="0">
+        <v>309</v>
+      </c>
+      <c r="K473" s="0"/>
+      <c r="L473" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="M473" s="0"/>
+    </row>
+    <row r="474">
+      <c r="A474" t="n" s="0">
+        <v>473.0</v>
+      </c>
+      <c r="B474" t="s" s="0">
+        <v>913</v>
+      </c>
+      <c r="C474" t="s" s="0">
+        <v>310</v>
+      </c>
+      <c r="D474" t="s" s="0">
+        <v>153</v>
+      </c>
+      <c r="E474" t="s" s="0">
+        <v>154</v>
+      </c>
+      <c r="F474" t="s" s="0">
+        <v>155</v>
+      </c>
+      <c r="G474" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="H474" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="I474" t="s" s="0">
+        <v>150</v>
+      </c>
+      <c r="J474" t="s" s="0">
+        <v>925</v>
+      </c>
+      <c r="K474" s="0"/>
+      <c r="L474" t="s" s="0">
+        <v>215</v>
+      </c>
+      <c r="M474" s="0"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>